<commit_message>
Cleaning data for 4 patients
</commit_message>
<xml_diff>
--- a/specification/Monitoring_Diagnosed_Patients_Endpoints_Matching_Synthea_Patients_rev1.xlsx
+++ b/specification/Monitoring_Diagnosed_Patients_Endpoints_Matching_Synthea_Patients_rev1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/73e59fead995feab/Desktop/DAP_HTN_Project/Bundle_files_for_logical_flow/Monitoring_Diagnosed_Patient/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Documents/GitHub/htnu18ig/specification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2489" documentId="8_{BE6B4F96-80A3-4251-9B5D-707635D151F9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{501AC0A8-E675-443E-B3A6-321E536B0F24}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCDDC5D-5D84-4E4C-93C6-CC9805522780}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="255" yWindow="180" windowWidth="17220" windowHeight="10410" xr2:uid="{716111E7-3C31-40E5-980D-4E4393A27B1B}"/>
+    <workbookView xWindow="30880" yWindow="-6560" windowWidth="36320" windowHeight="23500" xr2:uid="{716111E7-3C31-40E5-980D-4E4393A27B1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Monitoring_Diagnosed_Patient" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,6 @@
     <sheet name="Scratchwork" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1424,20 +1423,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F707CB2C-BA2E-4C7B-874E-A088081FC087}">
   <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="4" width="18.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" style="3" customWidth="1"/>
-    <col min="6" max="7" width="18.85546875" customWidth="1"/>
-    <col min="8" max="10" width="18.85546875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" customWidth="1"/>
+    <col min="2" max="4" width="18.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" style="3" customWidth="1"/>
+    <col min="6" max="7" width="18.83203125" customWidth="1"/>
+    <col min="8" max="10" width="18.83203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>43</v>
       </c>
@@ -1449,7 +1448,7 @@
       <c r="I1" s="9"/>
       <c r="J1" s="9"/>
     </row>
-    <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -1481,7 +1480,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -1513,7 +1512,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1545,7 +1544,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1577,7 +1576,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1607,7 +1606,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
@@ -1635,7 +1634,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>59</v>
       </c>
@@ -1657,7 +1656,7 @@
       </c>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>62</v>
       </c>
@@ -1677,7 +1676,7 @@
       </c>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:11" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" s="1" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>71</v>
       </c>
@@ -1695,7 +1694,7 @@
       </c>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:11" s="105" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" s="105" customFormat="1" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="102" t="s">
         <v>21</v>
       </c>
@@ -1727,7 +1726,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -1738,7 +1737,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
@@ -1770,7 +1769,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
         <v>4</v>
       </c>
@@ -1805,7 +1804,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="12"/>
       <c r="B15" s="12" t="s">
         <v>14</v>
@@ -1838,7 +1837,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
       <c r="B16" s="12" t="s">
         <v>14</v>
@@ -1866,7 +1865,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="12"/>
       <c r="B17" s="12" t="s">
         <v>14</v>
@@ -1892,7 +1891,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="12"/>
       <c r="B18" s="12" t="s">
         <v>14</v>
@@ -1906,7 +1905,7 @@
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
     </row>
-    <row r="19" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12"/>
       <c r="B19" s="12"/>
       <c r="C19" s="12"/>
@@ -1918,7 +1917,7 @@
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
     </row>
-    <row r="20" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12"/>
       <c r="B20" s="12" t="s">
         <v>14</v>
@@ -1931,7 +1930,7 @@
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
     </row>
-    <row r="21" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="12"/>
       <c r="B21" s="12" t="s">
         <v>14</v>
@@ -1945,8 +1944,8 @@
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
     </row>
-    <row r="22" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -1955,16 +1954,16 @@
       </c>
       <c r="E23"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B24" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C24" s="6"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -1974,7 +1973,7 @@
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -1983,7 +1982,7 @@
       </c>
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>11</v>
       </c>
@@ -1992,7 +1991,7 @@
       </c>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -2001,7 +2000,7 @@
       </c>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>17</v>
       </c>
@@ -2011,7 +2010,7 @@
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>19</v>
       </c>
@@ -2021,7 +2020,7 @@
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>20</v>
       </c>
@@ -2029,7 +2028,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -2037,7 +2036,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>108</v>
       </c>
@@ -2045,25 +2044,25 @@
         <v>109</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D36" s="6"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D37" s="6"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D38" s="6"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D39" s="6"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D40" s="6"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D41" s="6"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D42" s="6"/>
     </row>
   </sheetData>
@@ -2082,20 +2081,20 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="30"/>
-    <col min="3" max="3" width="9.140625" style="31"/>
-    <col min="4" max="4" width="9.140625" style="25"/>
-    <col min="5" max="5" width="9.7109375" style="32" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.7109375" style="33" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.7109375" style="44" bestFit="1" customWidth="1"/>
-    <col min="8" max="22" width="9.140625" style="21"/>
-    <col min="23" max="23" width="9.140625" style="25"/>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="30"/>
+    <col min="3" max="3" width="9.1640625" style="31"/>
+    <col min="4" max="4" width="9.1640625" style="25"/>
+    <col min="5" max="5" width="9.6640625" style="32" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.6640625" style="44" bestFit="1" customWidth="1"/>
+    <col min="8" max="22" width="9.1640625" style="21"/>
+    <col min="23" max="23" width="9.1640625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="40" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" s="40" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="51" t="s">
         <v>23</v>
       </c>
@@ -2160,7 +2159,7 @@
       <c r="V1" s="38"/>
       <c r="W1" s="39"/>
     </row>
-    <row r="2" spans="1:23" s="14" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" s="14" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="66"/>
       <c r="B2" s="46"/>
       <c r="C2" s="47"/>
@@ -2185,7 +2184,7 @@
       <c r="V2" s="21"/>
       <c r="W2" s="25"/>
     </row>
-    <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="92" t="s">
         <v>92</v>
       </c>
@@ -2196,7 +2195,7 @@
       <c r="F3" s="50"/>
       <c r="G3" s="41"/>
     </row>
-    <row r="4" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="93" t="s">
         <v>89</v>
       </c>
@@ -2258,7 +2257,7 @@
       <c r="V4" s="16"/>
       <c r="W4" s="37"/>
     </row>
-    <row r="5" spans="1:23" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" s="15" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="94" t="s">
         <v>91</v>
       </c>
@@ -2320,7 +2319,7 @@
       <c r="V5" s="26"/>
       <c r="W5" s="35"/>
     </row>
-    <row r="6" spans="1:23" s="14" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" s="14" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="67"/>
       <c r="B6" s="30"/>
       <c r="C6" s="31"/>
@@ -2335,7 +2334,7 @@
       <c r="V6" s="21"/>
       <c r="W6" s="31"/>
     </row>
-    <row r="7" spans="1:23" s="69" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" s="69" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="95" t="s">
         <v>93</v>
       </c>
@@ -2362,7 +2361,7 @@
       <c r="V7" s="21"/>
       <c r="W7" s="22"/>
     </row>
-    <row r="8" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="93" t="s">
         <v>88</v>
       </c>
@@ -2414,7 +2413,7 @@
       <c r="V8" s="16"/>
       <c r="W8" s="16"/>
     </row>
-    <row r="9" spans="1:23" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" s="15" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="94" t="s">
         <v>91</v>
       </c>
@@ -2466,14 +2465,14 @@
       <c r="V9" s="26"/>
       <c r="W9" s="26"/>
     </row>
-    <row r="10" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="20"/>
       <c r="C10" s="21"/>
       <c r="D10" s="22"/>
       <c r="E10" s="23"/>
       <c r="F10" s="24"/>
     </row>
-    <row r="11" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="92" t="s">
         <v>94</v>
       </c>
@@ -2484,7 +2483,7 @@
       <c r="F11" s="24"/>
       <c r="W11" s="31"/>
     </row>
-    <row r="12" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="93" t="s">
         <v>70</v>
       </c>
@@ -2532,7 +2531,7 @@
       <c r="V12" s="16"/>
       <c r="W12" s="16"/>
     </row>
-    <row r="13" spans="1:23" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="96" t="s">
         <v>91</v>
       </c>
@@ -2580,7 +2579,7 @@
       <c r="V13" s="65"/>
       <c r="W13" s="65"/>
     </row>
-    <row r="14" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="97" t="s">
         <v>69</v>
       </c>
@@ -2628,7 +2627,7 @@
       <c r="V14" s="21"/>
       <c r="W14" s="21"/>
     </row>
-    <row r="15" spans="1:23" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" s="15" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="94" t="s">
         <v>91</v>
       </c>
@@ -2676,8 +2675,8 @@
       <c r="V15" s="26"/>
       <c r="W15" s="26"/>
     </row>
-    <row r="16" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:23" s="69" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:23" s="69" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="95" t="s">
         <v>50</v>
       </c>
@@ -2704,7 +2703,7 @@
       <c r="V17" s="21"/>
       <c r="W17" s="21"/>
     </row>
-    <row r="18" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="93" t="s">
         <v>72</v>
       </c>
@@ -2770,7 +2769,7 @@
       <c r="V18" s="16"/>
       <c r="W18" s="37"/>
     </row>
-    <row r="19" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="97" t="s">
         <v>91</v>
       </c>
@@ -2836,7 +2835,7 @@
       <c r="V19" s="21"/>
       <c r="W19" s="31"/>
     </row>
-    <row r="20" spans="1:23" s="76" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="98" t="s">
         <v>73</v>
       </c>
@@ -2902,7 +2901,7 @@
       <c r="V20" s="77"/>
       <c r="W20" s="71"/>
     </row>
-    <row r="21" spans="1:23" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="96" t="s">
         <v>91</v>
       </c>
@@ -2968,7 +2967,7 @@
       <c r="V21" s="65"/>
       <c r="W21" s="59"/>
     </row>
-    <row r="22" spans="1:23" s="76" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" s="76" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="98" t="s">
         <v>74</v>
       </c>
@@ -3028,7 +3027,7 @@
       <c r="V22" s="77"/>
       <c r="W22" s="71"/>
     </row>
-    <row r="23" spans="1:23" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="96" t="s">
         <v>91</v>
       </c>
@@ -3088,7 +3087,7 @@
       <c r="V23" s="65"/>
       <c r="W23" s="59"/>
     </row>
-    <row r="24" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="97" t="s">
         <v>75</v>
       </c>
@@ -3148,7 +3147,7 @@
       <c r="V24" s="21"/>
       <c r="W24" s="31"/>
     </row>
-    <row r="25" spans="1:23" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" s="15" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="94" t="s">
         <v>91</v>
       </c>
@@ -3208,14 +3207,14 @@
       <c r="V25" s="26"/>
       <c r="W25" s="35"/>
     </row>
-    <row r="26" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="95" t="s">
         <v>95</v>
       </c>
       <c r="W27" s="31"/>
     </row>
-    <row r="28" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="93" t="s">
         <v>76</v>
       </c>
@@ -3277,7 +3276,7 @@
       <c r="V28" s="16"/>
       <c r="W28" s="37"/>
     </row>
-    <row r="29" spans="1:23" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="96" t="s">
         <v>91</v>
       </c>
@@ -3339,7 +3338,7 @@
       <c r="V29" s="65"/>
       <c r="W29" s="59"/>
     </row>
-    <row r="30" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="97" t="s">
         <v>77</v>
       </c>
@@ -3403,7 +3402,7 @@
       <c r="V30" s="21"/>
       <c r="W30" s="31"/>
     </row>
-    <row r="31" spans="1:23" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" s="15" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="94" t="s">
         <v>91</v>
       </c>
@@ -3467,13 +3466,13 @@
       <c r="V31" s="26"/>
       <c r="W31" s="35"/>
     </row>
-    <row r="32" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C32" s="21"/>
       <c r="D32" s="22"/>
       <c r="E32" s="23"/>
       <c r="F32" s="24"/>
     </row>
-    <row r="33" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="95" t="s">
         <v>61</v>
       </c>
@@ -3483,7 +3482,7 @@
       <c r="F33" s="24"/>
       <c r="W33" s="31"/>
     </row>
-    <row r="34" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="93" t="s">
         <v>78</v>
       </c>
@@ -3549,7 +3548,7 @@
       <c r="V34" s="16"/>
       <c r="W34" s="37"/>
     </row>
-    <row r="35" spans="1:23" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="96" t="s">
         <v>91</v>
       </c>
@@ -3615,7 +3614,7 @@
       <c r="V35" s="65"/>
       <c r="W35" s="59"/>
     </row>
-    <row r="36" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="97" t="s">
         <v>79</v>
       </c>
@@ -3679,7 +3678,7 @@
       <c r="V36" s="21"/>
       <c r="W36" s="31"/>
     </row>
-    <row r="37" spans="1:23" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="96" t="s">
         <v>91</v>
       </c>
@@ -3743,7 +3742,7 @@
       <c r="V37" s="65"/>
       <c r="W37" s="59"/>
     </row>
-    <row r="38" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="97" t="s">
         <v>80</v>
       </c>
@@ -3805,7 +3804,7 @@
       <c r="V38" s="21"/>
       <c r="W38" s="31"/>
     </row>
-    <row r="39" spans="1:23" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="96" t="s">
         <v>91</v>
       </c>
@@ -3867,7 +3866,7 @@
       <c r="V39" s="65"/>
       <c r="W39" s="59"/>
     </row>
-    <row r="40" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="97" t="s">
         <v>81</v>
       </c>
@@ -3931,7 +3930,7 @@
       <c r="V40" s="21"/>
       <c r="W40" s="31"/>
     </row>
-    <row r="41" spans="1:23" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:23" s="15" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="94" t="s">
         <v>91</v>
       </c>
@@ -3995,14 +3994,14 @@
       <c r="V41" s="26"/>
       <c r="W41" s="35"/>
     </row>
-    <row r="42" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="11"/>
       <c r="C42" s="21"/>
       <c r="D42" s="22"/>
       <c r="E42" s="23"/>
       <c r="F42" s="24"/>
     </row>
-    <row r="43" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="99" t="s">
         <v>64</v>
       </c>
@@ -4012,7 +4011,7 @@
       <c r="F43" s="24"/>
       <c r="W43" s="31"/>
     </row>
-    <row r="44" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="93" t="s">
         <v>82</v>
       </c>
@@ -4070,7 +4069,7 @@
       <c r="V44" s="16"/>
       <c r="W44" s="37"/>
     </row>
-    <row r="45" spans="1:23" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="96" t="s">
         <v>91</v>
       </c>
@@ -4128,7 +4127,7 @@
       <c r="V45" s="65"/>
       <c r="W45" s="59"/>
     </row>
-    <row r="46" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="97" t="s">
         <v>83</v>
       </c>
@@ -4192,7 +4191,7 @@
       <c r="V46" s="21"/>
       <c r="W46" s="31"/>
     </row>
-    <row r="47" spans="1:23" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:23" s="15" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="94" t="s">
         <v>91</v>
       </c>
@@ -4256,14 +4255,14 @@
       <c r="V47" s="26"/>
       <c r="W47" s="35"/>
     </row>
-    <row r="48" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="49" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="1:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="99" t="s">
         <v>65</v>
       </c>
       <c r="W49" s="31"/>
     </row>
-    <row r="50" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="93" t="s">
         <v>96</v>
       </c>
@@ -4321,7 +4320,7 @@
       <c r="V50" s="16"/>
       <c r="W50" s="37"/>
     </row>
-    <row r="51" spans="1:23" s="64" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" s="64" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="96" t="s">
         <v>91</v>
       </c>
@@ -4379,7 +4378,7 @@
       <c r="V51" s="65"/>
       <c r="W51" s="59"/>
     </row>
-    <row r="52" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="97" t="s">
         <v>84</v>
       </c>
@@ -4445,7 +4444,7 @@
       <c r="V52" s="21"/>
       <c r="W52" s="31"/>
     </row>
-    <row r="53" spans="1:23" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:23" s="15" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="94" t="s">
         <v>91</v>
       </c>
@@ -4511,12 +4510,12 @@
       <c r="V53" s="26"/>
       <c r="W53" s="35"/>
     </row>
-    <row r="54" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C54" s="21"/>
       <c r="D54" s="22"/>
       <c r="E54" s="23"/>
     </row>
-    <row r="55" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:23" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="93" t="s">
         <v>98</v>
       </c>
@@ -4525,7 +4524,7 @@
       <c r="E55" s="23"/>
       <c r="W55" s="31"/>
     </row>
-    <row r="56" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="93" t="s">
         <v>85</v>
       </c>
@@ -4593,7 +4592,7 @@
       <c r="V56" s="16"/>
       <c r="W56" s="37"/>
     </row>
-    <row r="57" spans="1:23" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:23" s="15" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="94" t="s">
         <v>91</v>
       </c>
@@ -4661,12 +4660,12 @@
       <c r="V57" s="26"/>
       <c r="W57" s="35"/>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B59" s="30" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A60" s="101" t="s">
         <v>99</v>
       </c>
@@ -4674,37 +4673,37 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B61" s="30" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B62" s="30" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B63" s="30" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.2">
       <c r="B64" s="30" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B65" s="30" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B66" s="30" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B67" s="30" t="s">
         <v>14</v>
       </c>
@@ -4724,9 +4723,9 @@
       <selection activeCell="D2" sqref="D2:D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>97</v>
       </c>
@@ -4737,7 +4736,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>97</v>
       </c>
@@ -4748,7 +4747,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>97</v>
       </c>
@@ -4759,7 +4758,7 @@
         <v>80.458075269298106</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>97</v>
       </c>
@@ -4770,7 +4769,7 @@
         <v>77.908910214761093</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>97</v>
       </c>
@@ -4781,7 +4780,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>97</v>
       </c>
@@ -4792,7 +4791,7 @@
         <v>82.0332325198262</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>97</v>
       </c>
@@ -4803,7 +4802,7 @@
         <v>75.776049558443304</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>97</v>
       </c>
@@ -4814,7 +4813,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>97</v>
       </c>
@@ -4825,7 +4824,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>97</v>
       </c>
@@ -4836,7 +4835,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>97</v>
       </c>
@@ -4847,7 +4846,7 @@
         <v>71.457348953771799</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>97</v>
       </c>
@@ -4858,7 +4857,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>97</v>
       </c>

</xml_diff>